<commit_message>
cm quality rule doc update in advance of 2021.8.0 release
</commit_message>
<xml_diff>
--- a/help/implementing/cloud-manager/assets/CodeQuality-rules-latest-CS.xlsx
+++ b/help/implementing/cloud-manager/assets/CodeQuality-rules-latest-CS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adobe-my.sharepoint.com/personal/jedelson_adobe_com/Documents/AMS/Pathlight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{66F76743-C75B-7A4F-8D1D-1800026AF33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2D6DCED-BF02-C543-8AC6-6B86A4986111}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{66F76743-C75B-7A4F-8D1D-1800026AF33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48FCA269-EBEE-424E-9FAF-C6A74825CA71}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1360" windowWidth="38400" windowHeight="14680" xr2:uid="{38B21097-AA8D-8C49-8C0F-A8DA08168C4C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="330">
   <si>
     <t>"@Deprecated" code should not be used</t>
   </si>
@@ -1003,6 +1003,18 @@
   </si>
   <si>
     <t>Index customizations of the damAssetLucene Oak index should be properly structured.</t>
+  </si>
+  <si>
+    <t>IndexAsyncProperty</t>
+  </si>
+  <si>
+    <t>IndexTikaNode</t>
+  </si>
+  <si>
+    <t>Custom Oak indexes must have a tika configuration</t>
+  </si>
+  <si>
+    <t>Custom Lucene Oak Indexes must not be synchronous</t>
   </si>
 </sst>
 </file>
@@ -1382,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B6A530D-317E-DF4C-BE2E-E97C27473266}">
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2008,75 +2020,78 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>318</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>319</v>
       </c>
       <c r="C37" t="s">
         <v>179</v>
       </c>
       <c r="D37" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E37" t="s">
-        <v>194</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>275</v>
+        <v>326</v>
       </c>
       <c r="B38" t="s">
-        <v>276</v>
+        <v>329</v>
       </c>
       <c r="C38" t="s">
         <v>179</v>
       </c>
       <c r="D38" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E38" t="s">
-        <v>230</v>
+        <v>291</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>270</v>
+        <v>327</v>
       </c>
       <c r="B39" t="s">
-        <v>271</v>
+        <v>328</v>
       </c>
       <c r="C39" t="s">
         <v>179</v>
       </c>
       <c r="D39" t="s">
-        <v>159</v>
+        <v>153</v>
+      </c>
+      <c r="E39" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>192</v>
+        <v>324</v>
       </c>
       <c r="B40" t="s">
-        <v>193</v>
+        <v>325</v>
       </c>
       <c r="C40" t="s">
         <v>179</v>
       </c>
       <c r="D40" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E40" t="s">
-        <v>191</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>189</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
-        <v>190</v>
+        <v>78</v>
       </c>
       <c r="C41" t="s">
         <v>179</v>
@@ -2085,15 +2100,15 @@
         <v>159</v>
       </c>
       <c r="E41" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>129</v>
+        <v>275</v>
       </c>
       <c r="B42" t="s">
-        <v>20</v>
+        <v>276</v>
       </c>
       <c r="C42" t="s">
         <v>179</v>
@@ -2102,15 +2117,15 @@
         <v>159</v>
       </c>
       <c r="E42" t="s">
-        <v>177</v>
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>270</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>271</v>
       </c>
       <c r="C43" t="s">
         <v>179</v>
@@ -2118,16 +2133,13 @@
       <c r="D43" t="s">
         <v>159</v>
       </c>
-      <c r="E43" t="s">
-        <v>186</v>
-      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>132</v>
+        <v>192</v>
       </c>
       <c r="B44" t="s">
-        <v>133</v>
+        <v>193</v>
       </c>
       <c r="C44" t="s">
         <v>179</v>
@@ -2136,21 +2148,21 @@
         <v>159</v>
       </c>
       <c r="E44" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="B45" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="C45" t="s">
         <v>179</v>
       </c>
       <c r="D45" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E45" t="s">
         <v>191</v>
@@ -2158,61 +2170,61 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>216</v>
+        <v>129</v>
       </c>
       <c r="B46" t="s">
-        <v>217</v>
+        <v>20</v>
       </c>
       <c r="C46" t="s">
         <v>179</v>
       </c>
       <c r="D46" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E46" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>224</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>225</v>
+        <v>63</v>
       </c>
       <c r="C47" t="s">
         <v>179</v>
       </c>
       <c r="D47" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E47" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>218</v>
+        <v>132</v>
       </c>
       <c r="B48" t="s">
-        <v>219</v>
+        <v>133</v>
       </c>
       <c r="C48" t="s">
         <v>179</v>
       </c>
       <c r="D48" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E48" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B49" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C49" t="s">
         <v>179</v>
@@ -2221,15 +2233,15 @@
         <v>171</v>
       </c>
       <c r="E49" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>216</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>217</v>
       </c>
       <c r="C50" t="s">
         <v>179</v>
@@ -2238,15 +2250,15 @@
         <v>171</v>
       </c>
       <c r="E50" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="C51" t="s">
         <v>179</v>
@@ -2255,15 +2267,15 @@
         <v>171</v>
       </c>
       <c r="E51" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>122</v>
+        <v>218</v>
       </c>
       <c r="B52" t="s">
-        <v>123</v>
+        <v>219</v>
       </c>
       <c r="C52" t="s">
         <v>179</v>
@@ -2272,15 +2284,15 @@
         <v>171</v>
       </c>
       <c r="E52" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>222</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>223</v>
       </c>
       <c r="C53" t="s">
         <v>179</v>
@@ -2289,29 +2301,32 @@
         <v>171</v>
       </c>
       <c r="E53" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="C54" t="s">
         <v>179</v>
       </c>
       <c r="D54" t="s">
         <v>171</v>
+      </c>
+      <c r="E54" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="C55" t="s">
         <v>179</v>
@@ -2320,15 +2335,15 @@
         <v>171</v>
       </c>
       <c r="E55" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
       <c r="C56" t="s">
         <v>179</v>
@@ -2337,15 +2352,15 @@
         <v>171</v>
       </c>
       <c r="E56" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>205</v>
+        <v>110</v>
       </c>
       <c r="B57" t="s">
-        <v>206</v>
+        <v>111</v>
       </c>
       <c r="C57" t="s">
         <v>179</v>
@@ -2354,32 +2369,29 @@
         <v>171</v>
       </c>
       <c r="E57" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
         <v>179</v>
       </c>
       <c r="D58" t="s">
         <v>171</v>
-      </c>
-      <c r="E58" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>195</v>
+        <v>28</v>
       </c>
       <c r="B59" t="s">
-        <v>196</v>
+        <v>29</v>
       </c>
       <c r="C59" t="s">
         <v>179</v>
@@ -2388,15 +2400,15 @@
         <v>171</v>
       </c>
       <c r="E59" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="C60" t="s">
         <v>179</v>
@@ -2405,15 +2417,15 @@
         <v>171</v>
       </c>
       <c r="E60" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B61" t="s">
-        <v>261</v>
+        <v>206</v>
       </c>
       <c r="C61" t="s">
         <v>179</v>
@@ -2422,15 +2434,15 @@
         <v>171</v>
       </c>
       <c r="E61" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="C62" t="s">
         <v>179</v>
@@ -2439,15 +2451,15 @@
         <v>171</v>
       </c>
       <c r="E62" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>195</v>
       </c>
       <c r="B63" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C63" t="s">
         <v>179</v>
@@ -2456,15 +2468,15 @@
         <v>171</v>
       </c>
       <c r="E63" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B64" t="s">
-        <v>259</v>
+        <v>80</v>
       </c>
       <c r="C64" t="s">
         <v>179</v>
@@ -2473,15 +2485,15 @@
         <v>171</v>
       </c>
       <c r="E64" t="s">
-        <v>260</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B65" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="C65" t="s">
         <v>179</v>
@@ -2495,10 +2507,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C66" t="s">
         <v>179</v>
@@ -2512,223 +2524,223 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>279</v>
+        <v>25</v>
       </c>
       <c r="B67" t="s">
-        <v>280</v>
+        <v>204</v>
       </c>
       <c r="C67" t="s">
         <v>179</v>
       </c>
       <c r="D67" t="s">
         <v>171</v>
+      </c>
+      <c r="E67" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>281</v>
+        <v>34</v>
       </c>
       <c r="B68" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="C68" t="s">
         <v>179</v>
       </c>
       <c r="D68" t="s">
         <v>171</v>
+      </c>
+      <c r="E68" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>283</v>
+        <v>210</v>
       </c>
       <c r="B69" t="s">
-        <v>284</v>
+        <v>211</v>
       </c>
       <c r="C69" t="s">
         <v>179</v>
       </c>
       <c r="D69" t="s">
         <v>171</v>
+      </c>
+      <c r="E69" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>324</v>
+        <v>86</v>
       </c>
       <c r="B70" t="s">
-        <v>325</v>
+        <v>87</v>
       </c>
       <c r="C70" t="s">
         <v>179</v>
       </c>
       <c r="D70" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E70" t="s">
-        <v>291</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F71" s="3"/>
+      <c r="A71" t="s">
+        <v>279</v>
+      </c>
+      <c r="B71" t="s">
+        <v>280</v>
+      </c>
+      <c r="C71" t="s">
+        <v>179</v>
+      </c>
+      <c r="D71" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>1</v>
+        <v>281</v>
       </c>
       <c r="B72" t="s">
-        <v>2</v>
+        <v>282</v>
       </c>
       <c r="C72" t="s">
         <v>179</v>
       </c>
       <c r="D72" t="s">
-        <v>175</v>
-      </c>
-      <c r="E72" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>283</v>
       </c>
       <c r="B73" t="s">
-        <v>65</v>
+        <v>284</v>
       </c>
       <c r="C73" t="s">
         <v>179</v>
       </c>
       <c r="D73" t="s">
-        <v>175</v>
-      </c>
-      <c r="E73" t="s">
-        <v>262</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>51</v>
-      </c>
-      <c r="B74" t="s">
-        <v>52</v>
-      </c>
-      <c r="C74" t="s">
-        <v>226</v>
-      </c>
-      <c r="D74" t="s">
-        <v>153</v>
-      </c>
-      <c r="E74" t="s">
-        <v>180</v>
-      </c>
+      <c r="A74" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F74" s="3"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="B75" t="s">
-        <v>107</v>
+        <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>226</v>
+        <v>179</v>
       </c>
       <c r="D75" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="E75" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>213</v>
+        <v>64</v>
       </c>
       <c r="B76" t="s">
-        <v>214</v>
+        <v>65</v>
       </c>
       <c r="C76" t="s">
-        <v>226</v>
+        <v>179</v>
       </c>
       <c r="D76" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="E76" t="s">
-        <v>215</v>
+        <v>262</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B77" t="s">
-        <v>251</v>
+        <v>52</v>
       </c>
       <c r="C77" t="s">
         <v>226</v>
       </c>
       <c r="D77" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E77" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="C78" t="s">
         <v>226</v>
       </c>
       <c r="D78" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E78" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>98</v>
+        <v>213</v>
       </c>
       <c r="B79" t="s">
-        <v>99</v>
+        <v>214</v>
       </c>
       <c r="C79" t="s">
         <v>226</v>
       </c>
       <c r="D79" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E79" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="B80" t="s">
-        <v>17</v>
+        <v>251</v>
       </c>
       <c r="C80" t="s">
         <v>226</v>
@@ -2737,15 +2749,15 @@
         <v>159</v>
       </c>
       <c r="E80" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="B81" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="C81" t="s">
         <v>226</v>
@@ -2754,15 +2766,15 @@
         <v>159</v>
       </c>
       <c r="E81" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="B82" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="C82" t="s">
         <v>226</v>
@@ -2771,15 +2783,15 @@
         <v>159</v>
       </c>
       <c r="E82" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>130</v>
+        <v>16</v>
       </c>
       <c r="B83" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C83" t="s">
         <v>226</v>
@@ -2788,66 +2800,66 @@
         <v>159</v>
       </c>
       <c r="E83" t="s">
-        <v>227</v>
+        <v>177</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B84" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C84" t="s">
         <v>226</v>
       </c>
       <c r="D84" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E84" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>254</v>
+        <v>47</v>
       </c>
       <c r="B85" t="s">
-        <v>255</v>
+        <v>48</v>
       </c>
       <c r="C85" t="s">
         <v>226</v>
       </c>
       <c r="D85" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E85" t="s">
-        <v>256</v>
+        <v>212</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B86" t="s">
-        <v>229</v>
+        <v>21</v>
       </c>
       <c r="C86" t="s">
         <v>226</v>
       </c>
       <c r="D86" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E86" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>131</v>
+        <v>43</v>
       </c>
       <c r="B87" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C87" t="s">
         <v>226</v>
@@ -2856,15 +2868,15 @@
         <v>171</v>
       </c>
       <c r="E87" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>55</v>
+        <v>254</v>
       </c>
       <c r="B88" t="s">
-        <v>56</v>
+        <v>255</v>
       </c>
       <c r="C88" t="s">
         <v>226</v>
@@ -2873,15 +2885,15 @@
         <v>171</v>
       </c>
       <c r="E88" t="s">
-        <v>203</v>
+        <v>256</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="B89" t="s">
-        <v>115</v>
+        <v>229</v>
       </c>
       <c r="C89" t="s">
         <v>226</v>
@@ -2890,15 +2902,15 @@
         <v>171</v>
       </c>
       <c r="E89" t="s">
-        <v>173</v>
+        <v>230</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="B90" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="C90" t="s">
         <v>226</v>
@@ -2907,15 +2919,15 @@
         <v>171</v>
       </c>
       <c r="E90" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="B91" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C91" t="s">
         <v>226</v>
@@ -2929,10 +2941,10 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="B92" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="C92" t="s">
         <v>226</v>
@@ -2941,15 +2953,15 @@
         <v>171</v>
       </c>
       <c r="E92" t="s">
-        <v>253</v>
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>200</v>
+        <v>112</v>
       </c>
       <c r="B93" t="s">
-        <v>201</v>
+        <v>113</v>
       </c>
       <c r="C93" t="s">
         <v>226</v>
@@ -2958,15 +2970,15 @@
         <v>171</v>
       </c>
       <c r="E93" t="s">
-        <v>202</v>
+        <v>252</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>231</v>
+        <v>14</v>
       </c>
       <c r="B94" t="s">
-        <v>232</v>
+        <v>15</v>
       </c>
       <c r="C94" t="s">
         <v>226</v>
@@ -2975,15 +2987,15 @@
         <v>171</v>
       </c>
       <c r="E94" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B95" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="C95" t="s">
         <v>226</v>
@@ -2992,15 +3004,15 @@
         <v>171</v>
       </c>
       <c r="E95" t="s">
-        <v>177</v>
+        <v>253</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>61</v>
+        <v>200</v>
       </c>
       <c r="B96" t="s">
-        <v>272</v>
+        <v>201</v>
       </c>
       <c r="C96" t="s">
         <v>226</v>
@@ -3009,66 +3021,66 @@
         <v>171</v>
       </c>
       <c r="E96" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>118</v>
+        <v>231</v>
       </c>
       <c r="B97" t="s">
-        <v>119</v>
+        <v>232</v>
       </c>
       <c r="C97" t="s">
         <v>226</v>
       </c>
       <c r="D97" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E97" t="s">
-        <v>194</v>
+        <v>233</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="B98" t="s">
-        <v>125</v>
+        <v>67</v>
       </c>
       <c r="C98" t="s">
         <v>226</v>
       </c>
       <c r="D98" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E98" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="B99" t="s">
-        <v>85</v>
+        <v>272</v>
       </c>
       <c r="C99" t="s">
         <v>226</v>
       </c>
       <c r="D99" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E99" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B100" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C100" t="s">
         <v>226</v>
@@ -3082,10 +3094,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>244</v>
+        <v>124</v>
       </c>
       <c r="B101" t="s">
-        <v>245</v>
+        <v>125</v>
       </c>
       <c r="C101" t="s">
         <v>226</v>
@@ -3094,15 +3106,15 @@
         <v>175</v>
       </c>
       <c r="E101" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>240</v>
+        <v>84</v>
       </c>
       <c r="B102" t="s">
-        <v>241</v>
+        <v>85</v>
       </c>
       <c r="C102" t="s">
         <v>226</v>
@@ -3111,16 +3123,15 @@
         <v>175</v>
       </c>
       <c r="E102" t="s">
-        <v>230</v>
-      </c>
-      <c r="F102" s="2"/>
+        <v>250</v>
+      </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>236</v>
+        <v>120</v>
       </c>
       <c r="B103" t="s">
-        <v>237</v>
+        <v>121</v>
       </c>
       <c r="C103" t="s">
         <v>226</v>
@@ -3129,15 +3140,15 @@
         <v>175</v>
       </c>
       <c r="E103" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B104" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C104" t="s">
         <v>226</v>
@@ -3151,10 +3162,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>273</v>
+        <v>240</v>
       </c>
       <c r="B105" t="s">
-        <v>274</v>
+        <v>241</v>
       </c>
       <c r="C105" t="s">
         <v>226</v>
@@ -3165,13 +3176,14 @@
       <c r="E105" t="s">
         <v>230</v>
       </c>
+      <c r="F105" s="2"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B106" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C106" t="s">
         <v>226</v>
@@ -3185,10 +3197,10 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="B107" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="C107" t="s">
         <v>226</v>
@@ -3202,10 +3214,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>242</v>
+        <v>273</v>
       </c>
       <c r="B108" t="s">
-        <v>243</v>
+        <v>274</v>
       </c>
       <c r="C108" t="s">
         <v>226</v>
@@ -3219,10 +3231,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B109" t="s">
-        <v>0</v>
+        <v>239</v>
       </c>
       <c r="C109" t="s">
         <v>226</v>
@@ -3231,15 +3243,15 @@
         <v>175</v>
       </c>
       <c r="E109" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>32</v>
+        <v>234</v>
       </c>
       <c r="B110" t="s">
-        <v>33</v>
+        <v>235</v>
       </c>
       <c r="C110" t="s">
         <v>226</v>
@@ -3248,15 +3260,15 @@
         <v>175</v>
       </c>
       <c r="E110" t="s">
-        <v>257</v>
+        <v>230</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>81</v>
+        <v>242</v>
       </c>
       <c r="B111" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="C111" t="s">
         <v>226</v>
@@ -3265,15 +3277,15 @@
         <v>175</v>
       </c>
       <c r="E111" t="s">
-        <v>180</v>
+        <v>230</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>3</v>
+        <v>248</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C112" t="s">
         <v>226</v>
@@ -3282,15 +3294,15 @@
         <v>175</v>
       </c>
       <c r="E112" t="s">
-        <v>198</v>
+        <v>249</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>285</v>
+        <v>32</v>
       </c>
       <c r="B113" t="s">
-        <v>297</v>
+        <v>33</v>
       </c>
       <c r="C113" t="s">
         <v>226</v>
@@ -3299,15 +3311,15 @@
         <v>175</v>
       </c>
       <c r="E113" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>286</v>
+        <v>81</v>
       </c>
       <c r="B114" t="s">
-        <v>296</v>
+        <v>258</v>
       </c>
       <c r="C114" t="s">
         <v>226</v>
@@ -3316,15 +3328,15 @@
         <v>175</v>
       </c>
       <c r="E114" t="s">
-        <v>291</v>
+        <v>180</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>287</v>
+        <v>3</v>
       </c>
       <c r="B115" t="s">
-        <v>295</v>
+        <v>4</v>
       </c>
       <c r="C115" t="s">
         <v>226</v>
@@ -3333,15 +3345,15 @@
         <v>175</v>
       </c>
       <c r="E115" t="s">
-        <v>291</v>
+        <v>198</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B116" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C116" t="s">
         <v>226</v>
@@ -3355,10 +3367,10 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B117" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C117" t="s">
         <v>226</v>
@@ -3372,10 +3384,10 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B118" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C118" t="s">
         <v>226</v>
@@ -3389,10 +3401,10 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="B119" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C119" t="s">
         <v>226</v>
@@ -3406,10 +3418,10 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="B120" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="C120" t="s">
         <v>226</v>
@@ -3423,10 +3435,10 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="B121" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="C121" t="s">
         <v>226</v>
@@ -3440,10 +3452,10 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B122" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C122" t="s">
         <v>226</v>
@@ -3457,10 +3469,10 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B123" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C123" t="s">
         <v>226</v>
@@ -3474,10 +3486,10 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B124" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C124" t="s">
         <v>226</v>
@@ -3491,10 +3503,10 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B125" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C125" t="s">
         <v>226</v>
@@ -3508,10 +3520,10 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B126" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C126" t="s">
         <v>226</v>
@@ -3525,10 +3537,10 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B127" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C127" t="s">
         <v>226</v>
@@ -3542,10 +3554,10 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B128" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C128" t="s">
         <v>226</v>
@@ -3559,10 +3571,10 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B129" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C129" t="s">
         <v>226</v>
@@ -3576,10 +3588,10 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B130" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C130" t="s">
         <v>226</v>
@@ -3593,35 +3605,69 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>134</v>
+        <v>320</v>
       </c>
       <c r="B131" t="s">
-        <v>135</v>
+        <v>321</v>
       </c>
       <c r="C131" t="s">
         <v>226</v>
       </c>
       <c r="D131" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="E131" t="s">
-        <v>228</v>
+        <v>291</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
+        <v>322</v>
+      </c>
+      <c r="B132" t="s">
+        <v>323</v>
+      </c>
+      <c r="C132" t="s">
+        <v>226</v>
+      </c>
+      <c r="D132" t="s">
+        <v>175</v>
+      </c>
+      <c r="E132" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>134</v>
+      </c>
+      <c r="B133" t="s">
+        <v>135</v>
+      </c>
+      <c r="C133" t="s">
+        <v>226</v>
+      </c>
+      <c r="D133" t="s">
+        <v>167</v>
+      </c>
+      <c r="E133" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>116</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B134" t="s">
         <v>117</v>
       </c>
-      <c r="C132" t="s">
-        <v>226</v>
-      </c>
-      <c r="D132" t="s">
+      <c r="C134" t="s">
+        <v>226</v>
+      </c>
+      <c r="D134" t="s">
         <v>167</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E134" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code quality rules and rel rating
</commit_message>
<xml_diff>
--- a/help/implementing/cloud-manager/assets/CodeQuality-rules-latest-CS.xlsx
+++ b/help/implementing/cloud-manager/assets/CodeQuality-rules-latest-CS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adobe-my.sharepoint.com/personal/jedelson_adobe_com/Documents/AMS/Pathlight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{66F76743-C75B-7A4F-8D1D-1800026AF33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48FCA269-EBEE-424E-9FAF-C6A74825CA71}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{66F76743-C75B-7A4F-8D1D-1800026AF33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C70E7FB7-2C1A-8D4E-B017-C7832267726A}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1360" windowWidth="38400" windowHeight="14680" xr2:uid="{38B21097-AA8D-8C49-8C0F-A8DA08168C4C}"/>
   </bookViews>
@@ -858,9 +858,6 @@
     <t>Product interfaces annotated with @ProviderType should not be implemented by custom code.</t>
   </si>
   <si>
-    <t>BannedPaths</t>
-  </si>
-  <si>
     <t>Customer packages should not install content under /libs</t>
   </si>
   <si>
@@ -1015,6 +1012,9 @@
   </si>
   <si>
     <t>Custom Lucene Oak Indexes must not be synchronous</t>
+  </si>
+  <si>
+    <t>BannedPath</t>
   </si>
 </sst>
 </file>
@@ -1397,7 +1397,7 @@
   <dimension ref="A1:F134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1989,10 +1989,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
       <c r="B35" t="s">
-        <v>278</v>
+        <v>300</v>
       </c>
       <c r="C35" t="s">
         <v>179</v>
@@ -2000,13 +2000,16 @@
       <c r="D35" t="s">
         <v>153</v>
       </c>
+      <c r="E35" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="B36" t="s">
-        <v>301</v>
+        <v>318</v>
       </c>
       <c r="C36" t="s">
         <v>179</v>
@@ -2015,15 +2018,15 @@
         <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="B37" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C37" t="s">
         <v>179</v>
@@ -2032,7 +2035,7 @@
         <v>153</v>
       </c>
       <c r="E37" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2040,7 +2043,7 @@
         <v>326</v>
       </c>
       <c r="B38" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C38" t="s">
         <v>179</v>
@@ -2049,15 +2052,15 @@
         <v>153</v>
       </c>
       <c r="E38" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B39" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C39" t="s">
         <v>179</v>
@@ -2066,24 +2069,21 @@
         <v>153</v>
       </c>
       <c r="E39" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="B40" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="C40" t="s">
         <v>179</v>
       </c>
       <c r="D40" t="s">
-        <v>153</v>
-      </c>
-      <c r="E40" t="s">
-        <v>291</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2592,10 +2592,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>278</v>
+      </c>
+      <c r="B71" t="s">
         <v>279</v>
-      </c>
-      <c r="B71" t="s">
-        <v>280</v>
       </c>
       <c r="C71" t="s">
         <v>179</v>
@@ -2606,10 +2606,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>280</v>
+      </c>
+      <c r="B72" t="s">
         <v>281</v>
-      </c>
-      <c r="B72" t="s">
-        <v>282</v>
       </c>
       <c r="C72" t="s">
         <v>179</v>
@@ -2620,10 +2620,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>282</v>
+      </c>
+      <c r="B73" t="s">
         <v>283</v>
-      </c>
-      <c r="B73" t="s">
-        <v>284</v>
       </c>
       <c r="C73" t="s">
         <v>179</v>
@@ -2634,10 +2634,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>299</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>179</v>
@@ -3350,10 +3350,10 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B116" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C116" t="s">
         <v>226</v>
@@ -3362,15 +3362,15 @@
         <v>175</v>
       </c>
       <c r="E116" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B117" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C117" t="s">
         <v>226</v>
@@ -3379,15 +3379,15 @@
         <v>175</v>
       </c>
       <c r="E117" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B118" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C118" t="s">
         <v>226</v>
@@ -3396,15 +3396,15 @@
         <v>175</v>
       </c>
       <c r="E118" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B119" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C119" t="s">
         <v>226</v>
@@ -3413,15 +3413,15 @@
         <v>175</v>
       </c>
       <c r="E119" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B120" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C120" t="s">
         <v>226</v>
@@ -3430,33 +3430,33 @@
         <v>175</v>
       </c>
       <c r="E120" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>289</v>
+      </c>
+      <c r="B121" t="s">
+        <v>291</v>
+      </c>
+      <c r="C121" t="s">
+        <v>226</v>
+      </c>
+      <c r="D121" t="s">
+        <v>175</v>
+      </c>
+      <c r="E121" t="s">
         <v>290</v>
-      </c>
-      <c r="B121" t="s">
-        <v>292</v>
-      </c>
-      <c r="C121" t="s">
-        <v>226</v>
-      </c>
-      <c r="D121" t="s">
-        <v>175</v>
-      </c>
-      <c r="E121" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>299</v>
+      </c>
+      <c r="B122" t="s">
         <v>300</v>
       </c>
-      <c r="B122" t="s">
-        <v>301</v>
-      </c>
       <c r="C122" t="s">
         <v>226</v>
       </c>
@@ -3464,16 +3464,16 @@
         <v>175</v>
       </c>
       <c r="E122" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>301</v>
+      </c>
+      <c r="B123" t="s">
         <v>302</v>
       </c>
-      <c r="B123" t="s">
-        <v>303</v>
-      </c>
       <c r="C123" t="s">
         <v>226</v>
       </c>
@@ -3481,16 +3481,16 @@
         <v>175</v>
       </c>
       <c r="E123" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
+        <v>303</v>
+      </c>
+      <c r="B124" t="s">
         <v>304</v>
       </c>
-      <c r="B124" t="s">
-        <v>305</v>
-      </c>
       <c r="C124" t="s">
         <v>226</v>
       </c>
@@ -3498,16 +3498,16 @@
         <v>175</v>
       </c>
       <c r="E124" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>305</v>
+      </c>
+      <c r="B125" t="s">
         <v>306</v>
       </c>
-      <c r="B125" t="s">
-        <v>307</v>
-      </c>
       <c r="C125" t="s">
         <v>226</v>
       </c>
@@ -3515,16 +3515,16 @@
         <v>175</v>
       </c>
       <c r="E125" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>307</v>
+      </c>
+      <c r="B126" t="s">
         <v>308</v>
       </c>
-      <c r="B126" t="s">
-        <v>309</v>
-      </c>
       <c r="C126" t="s">
         <v>226</v>
       </c>
@@ -3532,16 +3532,16 @@
         <v>175</v>
       </c>
       <c r="E126" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>309</v>
+      </c>
+      <c r="B127" t="s">
         <v>310</v>
       </c>
-      <c r="B127" t="s">
-        <v>311</v>
-      </c>
       <c r="C127" t="s">
         <v>226</v>
       </c>
@@ -3549,16 +3549,16 @@
         <v>175</v>
       </c>
       <c r="E127" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>311</v>
+      </c>
+      <c r="B128" t="s">
         <v>312</v>
       </c>
-      <c r="B128" t="s">
-        <v>313</v>
-      </c>
       <c r="C128" t="s">
         <v>226</v>
       </c>
@@ -3566,16 +3566,16 @@
         <v>175</v>
       </c>
       <c r="E128" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>313</v>
+      </c>
+      <c r="B129" t="s">
         <v>314</v>
       </c>
-      <c r="B129" t="s">
-        <v>315</v>
-      </c>
       <c r="C129" t="s">
         <v>226</v>
       </c>
@@ -3583,16 +3583,16 @@
         <v>175</v>
       </c>
       <c r="E129" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>315</v>
+      </c>
+      <c r="B130" t="s">
         <v>316</v>
       </c>
-      <c r="B130" t="s">
-        <v>317</v>
-      </c>
       <c r="C130" t="s">
         <v>226</v>
       </c>
@@ -3600,16 +3600,16 @@
         <v>175</v>
       </c>
       <c r="E130" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>319</v>
+      </c>
+      <c r="B131" t="s">
         <v>320</v>
       </c>
-      <c r="B131" t="s">
-        <v>321</v>
-      </c>
       <c r="C131" t="s">
         <v>226</v>
       </c>
@@ -3617,16 +3617,16 @@
         <v>175</v>
       </c>
       <c r="E131" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
+        <v>321</v>
+      </c>
+      <c r="B132" t="s">
         <v>322</v>
       </c>
-      <c r="B132" t="s">
-        <v>323</v>
-      </c>
       <c r="C132" t="s">
         <v>226</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>175</v>
       </c>
       <c r="E132" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>